<commit_message>
modifications to input data to help in data cleaning, renaming columns etc
</commit_message>
<xml_diff>
--- a/data/Renewables_CC_2011-2039.xlsx
+++ b/data/Renewables_CC_2011-2039.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Documents\UT_Grad\EDP_LAW379M\EnviroDev_Policy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EF292D-97EC-4B6B-8114-A49300B0D515}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CA8903-2449-4A6C-A8F9-F9AB6F8425D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E2AF5FF4-F4E9-4685-AE06-5CBBF82E0C69}"/>
   </bookViews>
@@ -38,13 +38,13 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Solar_PV</t>
+    <t>Extrapolated</t>
   </si>
   <si>
-    <t>Onshore_Wind</t>
+    <t>Solar_PV_Cost</t>
   </si>
   <si>
-    <t>Extrapolated</t>
+    <t>Onshore_Wind_Cost</t>
   </si>
 </sst>
 </file>
@@ -2324,7 +2324,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2334,13 +2334,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>